<commit_message>
Uploaded to Spira via GIT
</commit_message>
<xml_diff>
--- a/MxMasterTest/MxNavigation/b2180-MyAccount-MyExhibits/Main.rvl.xlsx
+++ b/MxMasterTest/MxNavigation/b2180-MyAccount-MyExhibits/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Flow</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>2000</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">

</xml_diff>